<commit_message>
corrections + added code for generating datasets
</commit_message>
<xml_diff>
--- a/data/TALD/standard_language_datapoints.xlsx
+++ b/data/TALD/standard_language_datapoints.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="91">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t xml:space="preserve">aff_col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataset_version</t>
   </si>
   <si>
     <t xml:space="preserve">Standard Armenian</t>
@@ -310,6 +307,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -397,8 +395,8 @@
   </sheetPr>
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V9" activeCellId="0" sqref="V9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W:W"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -473,13 +471,11 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="W1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>41.009625</v>
@@ -488,36 +484,36 @@
         <v>44.384086</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="T2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="U2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>40.977675</v>
@@ -526,33 +522,33 @@
         <v>46.4736975</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="V3" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>41.51572</v>
@@ -561,33 +557,33 @@
         <v>47.89507</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="I4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="T4" s="0" t="s">
+      <c r="U4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="0" t="s">
+      <c r="V4" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>41.61866</v>
@@ -596,33 +592,33 @@
         <v>47.32436</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="T5" s="0" t="s">
+      <c r="U5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="U5" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="V5" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>41.81574</v>
@@ -631,33 +627,33 @@
         <v>44.31883</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="I6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T6" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T6" s="0" t="s">
+      <c r="U6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="V6" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="U6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="V6" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>41.92418</v>
@@ -666,33 +662,33 @@
         <v>47.58429</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="T7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="U7" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>42.01976</v>
@@ -701,33 +697,33 @@
         <v>47.83791</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="T8" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="T8" s="0" t="s">
+      <c r="U8" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="U8" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="V8" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>42.13275</v>
@@ -736,33 +732,33 @@
         <v>47.0809</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="T9" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="T9" s="0" t="s">
+      <c r="U9" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="U9" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="V9" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>42.42568</v>
@@ -771,33 +767,33 @@
         <v>47.43876</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="T10" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="T10" s="0" t="s">
+      <c r="U10" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="U10" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="V10" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>42.43056</v>
@@ -806,33 +802,33 @@
         <v>46.66639</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="T11" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="T11" s="0" t="s">
+      <c r="U11" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="U11" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="V11" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>43</v>
@@ -841,33 +837,33 @@
         <v>47</v>
       </c>
       <c r="F12" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="H12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="T12" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="T12" s="0" t="s">
+      <c r="U12" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="U12" s="0" t="s">
+      <c r="V12" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="V12" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>43.16667</v>
@@ -876,33 +872,33 @@
         <v>44.81667</v>
       </c>
       <c r="F13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="H13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="T13" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="T13" s="0" t="s">
+      <c r="U13" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="U13" s="0" t="s">
+      <c r="V13" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="V13" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>43.5</v>
@@ -911,33 +907,33 @@
         <v>45.5</v>
       </c>
       <c r="F14" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="T14" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="T14" s="0" t="s">
+      <c r="U14" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="U14" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="V14" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>43.59168</v>
@@ -946,28 +942,28 @@
         <v>46.66178</v>
       </c>
       <c r="F15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="T15" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="T15" s="0" t="s">
-        <v>91</v>
-      </c>
       <c r="U15" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V15" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>